<commit_message>
:bug: correction bug du thread
</commit_message>
<xml_diff>
--- a/sample/résultats rapport + graphiques.xlsx
+++ b/sample/résultats rapport + graphiques.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Laura\cours\polytech\5a\s9\OVR - SMA\5A-SMA-Tri-Collectif\sample\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7636F955-2D41-4A48-A41F-3014F550635A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EC19DD9-31AD-4375-98FC-70BBC0118E88}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Agents" sheetId="1" r:id="rId1"/>
@@ -36769,7 +36769,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L48"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="L47" sqref="L47"/>
     </sheetView>
   </sheetViews>
@@ -48968,7 +48968,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:L48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
@@ -49927,7 +49927,7 @@
         <v>0.61184664029365865</v>
       </c>
       <c r="L31" s="4901">
-        <f t="shared" ref="L15:L48" si="2">B31/A19</f>
+        <f t="shared" ref="L31:L48" si="2">B31/A19</f>
         <v>0.97</v>
       </c>
     </row>
@@ -51385,7 +51385,7 @@
         <v>0.57511689654489107</v>
       </c>
       <c r="L31" s="4901">
-        <f t="shared" ref="L15:L48" si="2">C31/B19</f>
+        <f t="shared" ref="L31:L48" si="2">C31/B19</f>
         <v>0.99199999999999999</v>
       </c>
     </row>
@@ -52843,7 +52843,7 @@
         <v>0.58559969277210655</v>
       </c>
       <c r="L31" s="4901">
-        <f t="shared" ref="L15:L48" si="2">(B31+C31)/(A19+B19)</f>
+        <f t="shared" ref="L31:L48" si="2">(B31+C31)/(A19+B19)</f>
         <v>0.9830000000000001</v>
       </c>
     </row>

</xml_diff>

<commit_message>
:pencil: nombre de blocs rapport
</commit_message>
<xml_diff>
--- a/sample/résultats rapport + graphiques.xlsx
+++ b/sample/résultats rapport + graphiques.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Laura\cours\polytech\5a\s9\OVR - SMA\5A-SMA-Tri-Collectif\sample\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EC19DD9-31AD-4375-98FC-70BBC0118E88}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4BF5370-9C3F-4A5D-B514-C702346249ED}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Agents" sheetId="1" r:id="rId1"/>
@@ -25,6 +25,10 @@
     <sheet name="Grid Cols (M)" sheetId="10" r:id="rId10"/>
     <sheet name="Grid Rows (N)" sheetId="11" r:id="rId11"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">('Block A'!$A$2,'Block A'!$A$19,'Block A'!$A$36)</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">('Block A'!$E$14,'Block A'!$E$31,'Block A'!$E$48)</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -13747,24 +13751,37 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
             <c:numRef>
               <c:f>('Block A'!$A$2,'Block A'!$A$19,'Block A'!$A$36)</c:f>
               <c:numCache>
@@ -13781,8 +13798,8 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:cat>
-          <c:val>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
               <c:f>('Block A'!$E$14,'Block A'!$E$31,'Block A'!$E$48)</c:f>
               <c:numCache>
@@ -13799,7 +13816,8 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:yVal>
+          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-980E-4774-BFF3-A60DA12D4749}"/>
@@ -13814,12 +13832,10 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
         <c:axId val="975328944"/>
         <c:axId val="900226304"/>
-      </c:barChart>
-      <c:catAx>
+      </c:scatterChart>
+      <c:valAx>
         <c:axId val="975328944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
@@ -13865,11 +13881,8 @@
         </c:txPr>
         <c:crossAx val="900226304"/>
         <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
       <c:valAx>
         <c:axId val="900226304"/>
         <c:scaling>
@@ -13924,7 +13937,7 @@
         </c:txPr>
         <c:crossAx val="975328944"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -14050,24 +14063,37 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
             <c:numRef>
               <c:f>('Block A'!$A$2,'Block A'!$A$19,'Block A'!$A$36)</c:f>
               <c:numCache>
@@ -14084,8 +14110,8 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:cat>
-          <c:val>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
               <c:f>('Block A'!$H$14,'Block A'!$H$31,'Block A'!$H$48)</c:f>
               <c:numCache>
@@ -14102,7 +14128,8 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:yVal>
+          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-C918-42EC-BA52-3BC49BC198B7}"/>
@@ -14117,12 +14144,10 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
         <c:axId val="974443424"/>
         <c:axId val="978984752"/>
-      </c:barChart>
-      <c:catAx>
+      </c:scatterChart>
+      <c:valAx>
         <c:axId val="974443424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
@@ -14168,11 +14193,8 @@
         </c:txPr>
         <c:crossAx val="978984752"/>
         <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
       <c:valAx>
         <c:axId val="978984752"/>
         <c:scaling>
@@ -14227,7 +14249,7 @@
         </c:txPr>
         <c:crossAx val="974443424"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -36769,7 +36791,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A34" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="L47" sqref="L47"/>
     </sheetView>
   </sheetViews>
@@ -45637,7 +45659,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -46078,7 +46102,7 @@
         <v>99.2</v>
       </c>
       <c r="D14" s="1954">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D4:D13)</f>
         <v>0.53170621420198572</v>
       </c>
       <c r="E14" s="1955">
@@ -48968,8 +48992,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:L48"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I57" sqref="I57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -50426,8 +50450,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:L48"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+    <sheetView topLeftCell="A34" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J74" sqref="J57:J74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
:pencil: ajout de la partie sur taille de la grille
</commit_message>
<xml_diff>
--- a/sample/résultats rapport + graphiques.xlsx
+++ b/sample/résultats rapport + graphiques.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Laura\cours\polytech\5a\s9\OVR - SMA\5A-SMA-Tri-Collectif\sample\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4BF5370-9C3F-4A5D-B514-C702346249ED}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F75AD846-5591-4E14-9A45-2C9B5ACFF27D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="4" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Agents" sheetId="1" r:id="rId1"/>
@@ -26,8 +26,8 @@
     <sheet name="Grid Rows (N)" sheetId="11" r:id="rId11"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">('Block A'!$A$2,'Block A'!$A$19,'Block A'!$A$36)</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">('Block A'!$E$14,'Block A'!$E$31,'Block A'!$E$48)</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">('Grid Rows (N)'!$D$19,'Grid Rows (N)'!$D$2,'Grid Rows (N)'!$D$36)</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">('Grid Rows (N)'!$E$14,'Grid Rows (N)'!$E$31,'Grid Rows (N)'!$E$48)</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -17413,24 +17413,79 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
+            <a:ln w="25400" cap="rnd">
               <a:noFill/>
+              <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="log"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="0"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="fr-FR"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
             <c:numRef>
               <c:f>('Grid Cols (M)'!$E$19,'Grid Cols (M)'!$E$2,'Grid Cols (M)'!$E$36)</c:f>
               <c:numCache>
@@ -17447,8 +17502,8 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:cat>
-          <c:val>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
               <c:f>('Grid Cols (M)'!$G$31,'Grid Cols (M)'!$G$14,'Grid Cols (M)'!$G$48)</c:f>
               <c:numCache>
@@ -17465,7 +17520,8 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:yVal>
+          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-FCC2-41E6-AA0D-C59665E3C951}"/>
@@ -17480,12 +17536,10 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
         <c:axId val="779631872"/>
         <c:axId val="718192816"/>
-      </c:barChart>
-      <c:catAx>
+      </c:scatterChart>
+      <c:valAx>
         <c:axId val="779631872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
@@ -17531,11 +17585,8 @@
         </c:txPr>
         <c:crossAx val="718192816"/>
         <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
       <c:valAx>
         <c:axId val="718192816"/>
         <c:scaling>
@@ -17590,7 +17641,7 @@
         </c:txPr>
         <c:crossAx val="779631872"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -17716,24 +17767,79 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
+            <a:ln w="25400" cap="rnd">
               <a:noFill/>
+              <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="log"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="0"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="fr-FR"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
             <c:numRef>
               <c:f>('Grid Cols (M)'!$E$19,'Grid Cols (M)'!$E$2,'Grid Cols (M)'!$E$36)</c:f>
               <c:numCache>
@@ -17750,8 +17856,8 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:cat>
-          <c:val>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
               <c:f>('Grid Cols (M)'!$H$31,'Grid Cols (M)'!$H$14,'Grid Cols (M)'!$H$48)</c:f>
               <c:numCache>
@@ -17768,7 +17874,8 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:yVal>
+          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-EF7B-43BB-9683-D9960D90652A}"/>
@@ -17783,12 +17890,10 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
         <c:axId val="721084944"/>
         <c:axId val="896419888"/>
-      </c:barChart>
-      <c:catAx>
+      </c:scatterChart>
+      <c:valAx>
         <c:axId val="721084944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
@@ -17834,11 +17939,8 @@
         </c:txPr>
         <c:crossAx val="896419888"/>
         <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
       <c:valAx>
         <c:axId val="896419888"/>
         <c:scaling>
@@ -17893,7 +17995,7 @@
         </c:txPr>
         <c:crossAx val="721084944"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -18019,24 +18121,85 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
+            <a:ln w="25400" cap="rnd">
               <a:noFill/>
+              <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="log"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="0"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="1.0468066491688538E-3"/>
+                  <c:y val="-2.7036672499270924E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="fr-FR"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
             <c:numRef>
               <c:f>('Grid Rows (N)'!$D$19,'Grid Rows (N)'!$D$2,'Grid Rows (N)'!$D$36)</c:f>
               <c:numCache>
@@ -18053,8 +18216,8 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:cat>
-          <c:val>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
               <c:f>('Grid Rows (N)'!$G$31,'Grid Rows (N)'!$G$14,'Grid Rows (N)'!$G$48)</c:f>
               <c:numCache>
@@ -18071,7 +18234,8 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:yVal>
+          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-05AD-4B1A-9432-307D9916BFBA}"/>
@@ -18086,12 +18250,10 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
         <c:axId val="779640672"/>
         <c:axId val="775658624"/>
-      </c:barChart>
-      <c:catAx>
+      </c:scatterChart>
+      <c:valAx>
         <c:axId val="779640672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
@@ -18137,11 +18299,8 @@
         </c:txPr>
         <c:crossAx val="775658624"/>
         <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
       <c:valAx>
         <c:axId val="775658624"/>
         <c:scaling>
@@ -18196,7 +18355,7 @@
         </c:txPr>
         <c:crossAx val="779640672"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -18322,24 +18481,85 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
+            <a:ln w="25400" cap="rnd">
               <a:noFill/>
+              <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="log"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="0"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="3.8013998250218723E-4"/>
+                  <c:y val="2.909594634004083E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="fr-FR"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
             <c:numRef>
               <c:f>('Grid Rows (N)'!$D$19,'Grid Rows (N)'!$D$2,'Grid Rows (N)'!$D$36)</c:f>
               <c:numCache>
@@ -18356,8 +18576,8 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:cat>
-          <c:val>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
               <c:f>('Grid Rows (N)'!$H$31,'Grid Rows (N)'!$H$14,'Grid Rows (N)'!$H$48)</c:f>
               <c:numCache>
@@ -18374,7 +18594,8 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:yVal>
+          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-5A4B-4B02-8D12-3E124157991B}"/>
@@ -18389,12 +18610,10 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
         <c:axId val="973423664"/>
         <c:axId val="904068560"/>
-      </c:barChart>
-      <c:catAx>
+      </c:scatterChart>
+      <c:valAx>
         <c:axId val="973423664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
@@ -18440,11 +18659,8 @@
         </c:txPr>
         <c:crossAx val="904068560"/>
         <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
       <c:valAx>
         <c:axId val="904068560"/>
         <c:scaling>
@@ -18499,7 +18715,336 @@
         </c:txPr>
         <c:crossAx val="973423664"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart28.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="log"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="0"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="fr-FR"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>('Grid Rows (N)'!$D$19,'Grid Rows (N)'!$D$2,'Grid Rows (N)'!$D$36)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>('Grid Rows (N)'!$E$31,'Grid Rows (N)'!$E$14,'Grid Rows (N)'!$E$48)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>4.8899755501222489E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.4233611216369836E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.6705336329930348E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-C6FB-445A-960C-A6776BB303AE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1978696927"/>
+        <c:axId val="2077291215"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1978696927"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2077291215"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="2077291215"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1978696927"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -21517,12 +22062,9 @@
 </file>
 
 <file path=xl/charts/colors26.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="12">
   <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
   <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
   <a:schemeClr val="accent6"/>
   <cs:variation/>
   <cs:variation>
@@ -21557,6 +22099,43 @@
 </file>
 
 <file path=xl/charts/colors27.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="12">
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors28.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -31936,6 +32515,509 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style28.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -35616,6 +36698,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1926772</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>185056</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>174172</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>152399</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Graphique 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8C836CFD-5AA5-4068-B17E-E49AB9AF47F2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -38251,8 +39369,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:J48"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="J61" sqref="J61"/>
+    <sheetView topLeftCell="A41" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I65" sqref="I65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -39646,8 +40764,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:J48"/>
   <sheetViews>
-    <sheetView topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="I55" sqref="I55"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D68" sqref="D68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -48992,7 +50110,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:L48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A46" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="I57" sqref="I57"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
:pencil: ajout de la partie sur le nb d'agents
</commit_message>
<xml_diff>
--- a/sample/résultats rapport + graphiques.xlsx
+++ b/sample/résultats rapport + graphiques.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Laura\cours\polytech\5a\s9\OVR - SMA\5A-SMA-Tri-Collectif\sample\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F75AD846-5591-4E14-9A45-2C9B5ACFF27D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A62FDF46-E001-4A77-A9A5-B8603621964D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="4" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Agents" sheetId="1" r:id="rId1"/>
@@ -26,8 +26,10 @@
     <sheet name="Grid Rows (N)" sheetId="11" r:id="rId11"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">('Grid Rows (N)'!$D$19,'Grid Rows (N)'!$D$2,'Grid Rows (N)'!$D$36)</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">('Grid Rows (N)'!$E$14,'Grid Rows (N)'!$E$31,'Grid Rows (N)'!$E$48)</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">(Agents!$C$2,Agents!$C$19,Agents!$C$36)</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">(Agents!$E$14,Agents!$E$31,Agents!$E$48)</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">('Memory (t)'!$F$2,'Memory (t)'!$F$19,'Memory (t)'!$F$36)</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">('Memory (t)'!$G$14,'Memory (t)'!$G$31,'Memory (t)'!$G$48)</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -12515,24 +12517,79 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
+            <a:ln w="25400" cap="rnd">
               <a:noFill/>
+              <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="0"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="fr-FR"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
             <c:numRef>
               <c:f>(Agents!$C$2,Agents!$C$19,Agents!$C$36)</c:f>
               <c:numCache>
@@ -12549,8 +12606,8 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:cat>
-          <c:val>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
               <c:f>(Agents!$L$14,Agents!$L$31,Agents!$L$48)</c:f>
               <c:numCache>
@@ -12567,7 +12624,8 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:yVal>
+          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-9E0C-4127-B77E-E7F90CC31619}"/>
@@ -12582,12 +12640,10 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
         <c:axId val="709194576"/>
         <c:axId val="638709872"/>
-      </c:barChart>
-      <c:catAx>
+      </c:scatterChart>
+      <c:valAx>
         <c:axId val="709194576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
@@ -12633,11 +12689,8 @@
         </c:txPr>
         <c:crossAx val="638709872"/>
         <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
       <c:valAx>
         <c:axId val="638709872"/>
         <c:scaling>
@@ -12692,7 +12745,7 @@
         </c:txPr>
         <c:crossAx val="709194576"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -12781,11 +12834,11 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="fr-FR"/>
-              <a:t>Nombre de colonies en fonction de la taille</a:t>
+              <a:t>Proportion de blocs A voisins de blocs B en fonction du nombre de mouvements</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="fr-FR" baseline="0"/>
-              <a:t> de la mémoire</a:t>
+              <a:t> successifs</a:t>
             </a:r>
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
@@ -12823,62 +12876,76 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
             <c:numRef>
-              <c:f>('Memory (t)'!$F$2,'Memory (t)'!$F$19,'Memory (t)'!$F$36)</c:f>
+              <c:f>('Moves (i)'!$G$2,'Moves (i)'!$G$19,'Moves (i)'!$G$36)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>15</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>50</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:cat>
-          <c:val>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
-              <c:f>('Memory (t)'!$G$14,'Memory (t)'!$G$31,'Memory (t)'!$G$48)</c:f>
+              <c:f>('Moves (i)'!$E$14,'Moves (i)'!$E$31,'Moves (i)'!$E$48)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>26.6</c:v>
+                  <c:v>4.5464003329171868E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>28.6</c:v>
+                  <c:v>0.43789431487426284</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>31.2</c:v>
+                  <c:v>0.50460321215764226</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:yVal>
+          <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-5EEF-431F-9321-686C742C77EA}"/>
+              <c16:uniqueId val="{00000000-3B22-4519-A915-C4288E9F46CB}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -12890,13 +12957,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
-        <c:axId val="905160624"/>
-        <c:axId val="640102272"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="905160624"/>
+        <c:axId val="916507472"/>
+        <c:axId val="916330288"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="916507472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12939,15 +13004,12 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="640102272"/>
+        <c:crossAx val="916330288"/>
         <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
       <c:valAx>
-        <c:axId val="640102272"/>
+        <c:axId val="916330288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12998,9 +13060,9 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="905160624"/>
+        <c:crossAx val="916507472"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -13061,10 +13123,369 @@
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
+      <c14:style val="106"/>
     </mc:Choice>
     <mc:Fallback>
-      <c:style val="2"/>
+      <c:style val="6"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="fr-FR"/>
+              <a:t>Nombre de colonies en fonction de la taille</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="fr-FR" baseline="0"/>
+              <a:t> de la mémoire</a:t>
+            </a:r>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="log"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="0"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="fr-FR"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>('Memory (t)'!$F$2,'Memory (t)'!$F$19,'Memory (t)'!$F$36)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>50</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>('Memory (t)'!$G$14,'Memory (t)'!$G$31,'Memory (t)'!$G$48)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>26.6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>28.6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>31.2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5EEF-431F-9321-686C742C77EA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="905160624"/>
+        <c:axId val="640102272"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="905160624"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="640102272"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="640102272"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="905160624"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="106"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="6"/>
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
@@ -13140,7 +13561,7 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="accent4"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -13151,11 +13572,11 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="accent4"/>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent1"/>
+                  <a:schemeClr val="accent4"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -13371,7 +13792,367 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="106"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="6"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Taille moyenne d'une colonie en fonction de la taille de la mémoire</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="log"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="0"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-3.5825896762904638E-2"/>
+                  <c:y val="1.0266841644794401E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="fr-FR"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>('Memory (t)'!$F$2,'Memory (t)'!$F$19,'Memory (t)'!$F$36)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>50</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>('Memory (t)'!$H$14,'Memory (t)'!$H$31,'Memory (t)'!$H$48)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>7.46863745016105</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.0499934640705089</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.3565779143198498</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6A1D-47F2-B1B5-43625BAA5B9A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1978329935"/>
+        <c:axId val="1750093023"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1978329935"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1750093023"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1750093023"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1978329935"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="fr-FR"/>
@@ -13679,7 +14460,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="fr-FR"/>
@@ -13991,7 +14772,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="fr-FR"/>
@@ -14303,7 +15084,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="fr-FR"/>
@@ -14611,7 +15392,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart18.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="fr-FR"/>
@@ -14914,7 +15695,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart19.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="fr-FR"/>
@@ -15217,7 +15998,312 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="fr-FR"/>
+              <a:t>Taille moyenne d'une colonie en fonction du nombre d'agents</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>(Agents!$C$2,Agents!$C$19,Agents!$C$36)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>(Agents!$H$14,Agents!$H$31,Agents!$H$48)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>7.4439666040754968</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.2727891473978401</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.8117375991491427</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-7BB5-4872-B05A-145F379ABA70}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="641208048"/>
+        <c:axId val="696110944"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="641208048"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="696110944"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="696110944"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="641208048"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart20.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="fr-FR"/>
@@ -15520,7 +16606,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart21.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="fr-FR"/>
@@ -15823,303 +16909,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="fr-FR"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="fr-FR"/>
-              <a:t>Taille moyenne d'une colonie en fonction du nombre d'agents</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="fr-FR"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:numRef>
-              <c:f>(Agents!$C$2,Agents!$C$19,Agents!$C$36)</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>100</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>(Agents!$H$14,Agents!$H$31,Agents!$H$48)</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>7.4439666040754968</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>7.2727891473978401</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>6.8117375991491427</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-7BB5-4872-B05A-145F379ABA70}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
-        <c:axId val="641208048"/>
-        <c:axId val="696110944"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="641208048"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="696110944"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="696110944"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="641208048"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="fr-FR"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart22.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="fr-FR"/>
@@ -16436,7 +17226,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart23.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="fr-FR"/>
@@ -16744,7 +17534,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart24.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="fr-FR"/>
@@ -17052,7 +17842,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart25.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="fr-FR"/>
@@ -17341,7 +18131,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart26.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="fr-FR"/>
@@ -17695,7 +18485,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart27.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="fr-FR"/>
@@ -18049,7 +18839,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart28.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="fr-FR"/>
@@ -18409,7 +19199,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart29.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="fr-FR"/>
@@ -18769,7 +19559,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="fr-FR"/>
@@ -18784,6 +19574,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Proportion de blocs A voisins de blocs B en fonction du nombre d'agents</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -18823,8 +19638,10 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -18834,71 +19651,27 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="accent6"/>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent1"/>
+                  <a:schemeClr val="accent6"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="log"/>
-            <c:dispRSqr val="1"/>
-            <c:dispEq val="0"/>
-            <c:trendlineLbl>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="fr-FR"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
-          </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>('Grid Rows (N)'!$D$19,'Grid Rows (N)'!$D$2,'Grid Rows (N)'!$D$36)</c:f>
+              <c:f>(Agents!$C$2,Agents!$C$19,Agents!$C$36)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>40</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>50</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>100</c:v>
@@ -18908,18 +19681,18 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>('Grid Rows (N)'!$E$31,'Grid Rows (N)'!$E$14,'Grid Rows (N)'!$E$48)</c:f>
+              <c:f>(Agents!$E$14,Agents!$E$31,Agents!$E$48)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>4.8899755501222489E-4</c:v>
+                  <c:v>2.1739130434782609E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.4233611216369836E-3</c:v>
+                  <c:v>2.1027857357998917E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.6705336329930348E-3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -18927,7 +19700,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-C6FB-445A-960C-A6776BB303AE}"/>
+              <c16:uniqueId val="{00000000-5A3B-427A-BD60-A5D3F682A360}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -18939,11 +19712,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1978696927"/>
-        <c:axId val="2077291215"/>
+        <c:axId val="1868806239"/>
+        <c:axId val="1869078799"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1978696927"/>
+        <c:axId val="1868806239"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -18986,12 +19759,12 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2077291215"/>
+        <c:crossAx val="1869078799"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2077291215"/>
+        <c:axId val="1869078799"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -19042,7 +19815,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1978696927"/>
+        <c:crossAx val="1868806239"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -19098,7 +19871,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="fr-FR"/>
@@ -19436,7 +20209,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="fr-FR"/>
@@ -19791,7 +20564,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="fr-FR"/>
@@ -20105,7 +20878,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="fr-FR"/>
@@ -20413,7 +21186,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="fr-FR"/>
@@ -20716,7 +21489,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="fr-FR"/>
@@ -21024,331 +21797,11 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="fr-FR"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="fr-FR"/>
-              <a:t>Proportion de blocs A voisins de blocs B en fonction du nombre de mouvements</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="fr-FR" baseline="0"/>
-              <a:t> successifs</a:t>
-            </a:r>
-            <a:endParaRPr lang="fr-FR"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="fr-FR"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="smoothMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>('Moves (i)'!$G$2,'Moves (i)'!$G$19,'Moves (i)'!$G$36)</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>10</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>('Moves (i)'!$E$14,'Moves (i)'!$E$31,'Moves (i)'!$E$48)</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>4.5464003329171868E-3</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.43789431487426284</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.50460321215764226</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-3B22-4519-A915-C4288E9F46CB}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="916507472"/>
-        <c:axId val="916330288"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="916507472"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="916330288"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="916330288"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="916507472"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="fr-FR"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="13">
+  <a:schemeClr val="accent6"/>
+  <a:schemeClr val="accent5"/>
   <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
   <cs:variation/>
   <cs:variation>
     <a:lumMod val="60000"/>
@@ -21422,122 +21875,20 @@
 </file>
 
 <file path=xl/charts/colors11.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinear" id="17">
   <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
 </cs:colorStyle>
 </file>
 
 <file path=xl/charts/colors12.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinear" id="17">
   <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
 </cs:colorStyle>
 </file>
 
 <file path=xl/charts/colors13.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinear" id="17">
   <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
 </cs:colorStyle>
 </file>
 
@@ -21782,13 +22133,10 @@
 </file>
 
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="13">
+  <a:schemeClr val="accent6"/>
+  <a:schemeClr val="accent5"/>
   <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
   <cs:variation/>
   <cs:variation>
     <a:lumMod val="60000"/>
@@ -22062,80 +22410,6 @@
 </file>
 
 <file path=xl/charts/colors26.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="12">
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/colors27.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="12">
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/colors28.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -22175,7 +22449,7 @@
 </cs:colorStyle>
 </file>
 
-<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/colors27.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -22183,6 +22457,117 @@
   <a:schemeClr val="accent4"/>
   <a:schemeClr val="accent5"/>
   <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors28.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="12">
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors29.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="12">
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="13">
+  <a:schemeClr val="accent6"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent4"/>
   <cs:variation/>
   <cs:variation>
     <a:lumMod val="60000"/>
@@ -33018,7 +33403,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style29.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -33521,8 +33906,8 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -33549,8 +33934,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -33651,6 +34036,1012 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
       <a:ln w="19050" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -34037,7 +35428,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -34540,7 +35931,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -35043,7 +36434,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -35546,7 +36937,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style9.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -36049,509 +37440,6 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style9.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -36559,13 +37447,13 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>381001</xdr:colOff>
       <xdr:row>50</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:rowOff>108857</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>185058</xdr:colOff>
       <xdr:row>67</xdr:row>
-      <xdr:rowOff>32655</xdr:rowOff>
+      <xdr:rowOff>65312</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -36621,6 +37509,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1578428</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>43543</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>283028</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>10886</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Graphique 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D047A218-20E9-4B77-807B-E40E82A699BB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -36698,42 +37622,6 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>1926772</xdr:colOff>
-      <xdr:row>50</xdr:row>
-      <xdr:rowOff>185056</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>174172</xdr:colOff>
-      <xdr:row>65</xdr:row>
-      <xdr:rowOff>152399</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Graphique 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8C836CFD-5AA5-4068-B17E-E49AB9AF47F2}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -37078,6 +37966,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>304801</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>97970</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>65313</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Graphique 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2863338E-EE89-4455-B841-B4DF51F8AFE9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -37909,8 +38833,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L48"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L47" sqref="L47"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J76" sqref="J76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -40764,7 +41688,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:J48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A34" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="D68" sqref="D68"/>
     </sheetView>
   </sheetViews>
@@ -48715,8 +49639,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:J48"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="O52" sqref="O52"/>
+    <sheetView tabSelected="1" topLeftCell="I13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Z44" sqref="Z44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
:pencil: ajout de la partie mémoire
</commit_message>
<xml_diff>
--- a/sample/résultats rapport + graphiques.xlsx
+++ b/sample/résultats rapport + graphiques.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Laura\cours\polytech\5a\s9\OVR - SMA\5A-SMA-Tri-Collectif\sample\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A62FDF46-E001-4A77-A9A5-B8603621964D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2BBDB3C-906B-4B76-A5E2-8DB717929C2F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,12 +25,6 @@
     <sheet name="Grid Cols (M)" sheetId="10" r:id="rId10"/>
     <sheet name="Grid Rows (N)" sheetId="11" r:id="rId11"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">(Agents!$C$2,Agents!$C$19,Agents!$C$36)</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">(Agents!$E$14,Agents!$E$31,Agents!$E$48)</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">('Memory (t)'!$F$2,'Memory (t)'!$F$19,'Memory (t)'!$F$36)</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">('Memory (t)'!$G$14,'Memory (t)'!$G$31,'Memory (t)'!$G$48)</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -37901,16 +37895,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>464127</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>1</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1139042</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>163287</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>159327</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>41564</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>1868384</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>19793</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -37937,16 +37931,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>519545</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>138545</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>127659</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>160317</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>214745</xdr:colOff>
-      <xdr:row>49</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>182088</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>21772</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -37973,16 +37967,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>304801</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>97970</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>457201</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>163285</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>1</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>65313</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>990601</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>130628</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -49639,7 +49633,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:J48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="Z44" sqref="Z44"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
:pencil: ajout partie sur K+
</commit_message>
<xml_diff>
--- a/sample/résultats rapport + graphiques.xlsx
+++ b/sample/résultats rapport + graphiques.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Laura\cours\polytech\5a\s9\OVR - SMA\5A-SMA-Tri-Collectif\sample\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2BBDB3C-906B-4B76-A5E2-8DB717929C2F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66AA4DD1-2803-46C0-B2BB-F0FB279A46D6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Agents" sheetId="1" r:id="rId1"/>
@@ -25,6 +25,10 @@
     <sheet name="Grid Cols (M)" sheetId="10" r:id="rId10"/>
     <sheet name="Grid Rows (N)" sheetId="11" r:id="rId11"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">('K+'!$E$14,'K+'!$E$31,'K+'!$E$48,'K+'!$E$65)</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">('K+'!$I$2,'K+'!$I$19,'K+'!$I$36,'K+'!$I$53)</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -20565,10 +20569,10 @@
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
+      <c14:style val="105"/>
     </mc:Choice>
     <mc:Fallback>
-      <c:style val="2"/>
+      <c:style val="5"/>
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
@@ -20635,24 +20639,37 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
             <c:numRef>
               <c:f>('K+'!$I$2,'K+'!$I$19,'K+'!$I$36,'K+'!$I$53)</c:f>
               <c:numCache>
@@ -20672,8 +20689,8 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:cat>
-          <c:val>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
               <c:f>('K+'!$E$14,'K+'!$E$31,'K+'!$E$48,'K+'!$E$65)</c:f>
               <c:numCache>
@@ -20693,7 +20710,8 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:yVal>
+          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-40B3-450C-88A9-9BD16D07A886}"/>
@@ -20708,12 +20726,10 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
         <c:axId val="896841712"/>
         <c:axId val="911075504"/>
-      </c:barChart>
-      <c:catAx>
+      </c:scatterChart>
+      <c:valAx>
         <c:axId val="896841712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
@@ -20759,11 +20775,8 @@
         </c:txPr>
         <c:crossAx val="911075504"/>
         <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
       <c:valAx>
         <c:axId val="911075504"/>
         <c:scaling>
@@ -20818,7 +20831,7 @@
         </c:txPr>
         <c:crossAx val="896841712"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -22675,42 +22688,8 @@
 </file>
 
 <file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinear" id="16">
   <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
 </cs:colorStyle>
 </file>
 
@@ -43077,7 +43056,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J99"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView topLeftCell="A82" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="K109" sqref="K109"/>
     </sheetView>
   </sheetViews>
@@ -45843,8 +45822,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J65"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="O32" sqref="O32"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="J83" sqref="J83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -49633,7 +49612,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:J48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A34" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="Z44" sqref="Z44"/>
     </sheetView>
   </sheetViews>
@@ -53944,7 +53923,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:L48"/>
   <sheetViews>
-    <sheetView topLeftCell="A58" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A52" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="J73" sqref="J73"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
:pencil: ajout de la partie sur l'erreur
</commit_message>
<xml_diff>
--- a/sample/résultats rapport + graphiques.xlsx
+++ b/sample/résultats rapport + graphiques.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Laura\cours\polytech\5a\s9\OVR - SMA\5A-SMA-Tri-Collectif\sample\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66AA4DD1-2803-46C0-B2BB-F0FB279A46D6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27E64C1F-1914-401F-9979-44E4F00A55F3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Agents" sheetId="1" r:id="rId1"/>
@@ -26,8 +26,11 @@
     <sheet name="Grid Rows (N)" sheetId="11" r:id="rId11"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">('K+'!$E$14,'K+'!$E$31,'K+'!$E$48,'K+'!$E$65)</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">('K+'!$I$2,'K+'!$I$19,'K+'!$I$36,'K+'!$I$53)</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">('Error (e)'!$G$14,'Error (e)'!$G$31,'Error (e)'!$G$48,'Error (e)'!$G$65,'Error (e)'!$G$82,'Error (e)'!$G$99)</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">('Error (e)'!$J$2,'Error (e)'!$J$19,'Error (e)'!$J$36,'Error (e)'!$J$53,'Error (e)'!$J$70,'Error (e)'!$J$87)</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">('K-'!$H$14,'K-'!$H$31,'K-'!$H$48)</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">('K-'!$H$2,'K-'!$H$19,'K-'!$H$36)</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">('K-'!$H$14,'K-'!$H$31,'K-'!$H$48)</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -12832,6 +12835,323 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="fr-FR"/>
+              <a:t>Taille</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="fr-FR" baseline="0"/>
+              <a:t> moyenne d'une colonie en fonction du nombre de mouvements successifs</a:t>
+            </a:r>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="C00000"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="C00000"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:srgbClr val="C00000"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>('Moves (i)'!$G$2,'Moves (i)'!$G$19,'Moves (i)'!$G$36)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>('Moves (i)'!$H$14,'Moves (i)'!$H$31,'Moves (i)'!$H$48)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>7.7870032305275938</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.6819178241816435</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.6208390158958212</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-531F-4778-85A8-AED9AE2DF008}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="896834112"/>
+        <c:axId val="900187984"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="896834112"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="900187984"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="900187984"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="896834112"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="fr-FR"/>
               <a:t>Proportion de blocs A voisins de blocs B en fonction du nombre de mouvements</a:t>
             </a:r>
             <a:r>
@@ -12875,7 +13195,7 @@
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
-        <c:scatterStyle val="smoothMarker"/>
+        <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -12883,7 +13203,7 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:srgbClr val="C00000"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -12894,11 +13214,11 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:srgbClr val="C00000"/>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent1"/>
+                  <a:srgbClr val="C00000"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -12940,7 +13260,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="1"/>
+          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-3B22-4519-A915-C4288E9F46CB}"/>
@@ -13114,7 +13434,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="fr-FR"/>
@@ -13473,7 +13793,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="fr-FR"/>
@@ -13790,7 +14110,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="fr-FR"/>
@@ -14150,7 +14470,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="fr-FR"/>
@@ -14458,7 +14778,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="fr-FR"/>
@@ -14770,7 +15090,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="fr-FR"/>
@@ -15082,7 +15402,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart18.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="fr-FR"/>
@@ -15390,7 +15710,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart19.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="fr-FR"/>
@@ -15638,309 +15958,6 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="774598992"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="fr-FR"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart19.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="fr-FR"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="fr-FR"/>
-              <a:t>Proportion de blocs A voisins de blocs B en fonction du nombre de blocs B</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="fr-FR"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:numRef>
-              <c:f>('Block B'!$B$2,'Block B'!$B$19,'Block B'!$B$36)</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>300</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>('Block B'!$E$14,'Block B'!$E$31,'Block B'!$E$48)</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2.3684210526315791E-3</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.8307616830938934E-2</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-4ACB-4538-9688-20634657074C}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
-        <c:axId val="974448224"/>
-        <c:axId val="978988912"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="974448224"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="978988912"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="978988912"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="974448224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -16336,6 +16353,309 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="fr-FR"/>
+              <a:t>Proportion de blocs A voisins de blocs B en fonction du nombre de blocs B</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>('Block B'!$B$2,'Block B'!$B$19,'Block B'!$B$36)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>300</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>('Block B'!$E$14,'Block B'!$E$31,'Block B'!$E$48)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.3684210526315791E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.8307616830938934E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4ACB-4538-9688-20634657074C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="974448224"/>
+        <c:axId val="978988912"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="974448224"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="978988912"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="978988912"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="974448224"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart21.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="fr-FR"/>
               <a:t>Nombre de colonies en fonction du nombre de blocs B</a:t>
             </a:r>
           </a:p>
@@ -16604,7 +16924,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart22.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="fr-FR"/>
@@ -16907,7 +17227,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart23.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="fr-FR"/>
@@ -16993,7 +17313,7 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:srgbClr val="002060"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -17004,11 +17324,11 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:srgbClr val="002060"/>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent1"/>
+                  <a:srgbClr val="002060"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -17224,7 +17544,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart24.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="fr-FR"/>
@@ -17301,24 +17621,77 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
+            <a:ln w="25400" cap="rnd">
               <a:noFill/>
+              <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="002060"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:srgbClr val="002060"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="0"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="fr-FR"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
             <c:numRef>
               <c:f>('K-'!$H$2,'K-'!$H$19,'K-'!$H$36)</c:f>
               <c:numCache>
@@ -17335,8 +17708,8 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:cat>
-          <c:val>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
               <c:f>('K-'!$L$14,'K-'!$L$31,'K-'!$L$48)</c:f>
               <c:numCache>
@@ -17353,7 +17726,8 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:yVal>
+          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-94F8-4B22-8C05-AECF91D56451}"/>
@@ -17368,12 +17742,10 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
         <c:axId val="782356832"/>
         <c:axId val="697588144"/>
-      </c:barChart>
-      <c:catAx>
+      </c:scatterChart>
+      <c:valAx>
         <c:axId val="782356832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
@@ -17419,11 +17791,8 @@
         </c:txPr>
         <c:crossAx val="697588144"/>
         <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
       <c:valAx>
         <c:axId val="697588144"/>
         <c:scaling>
@@ -17478,315 +17847,7 @@
         </c:txPr>
         <c:crossAx val="782356832"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="fr-FR"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart24.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="fr-FR"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="fr-FR"/>
-              <a:t>Nombre de colonies en fonction</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="fr-FR" baseline="0"/>
-              <a:t> de K -</a:t>
-            </a:r>
-            <a:endParaRPr lang="fr-FR"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="fr-FR"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:numRef>
-              <c:f>('K-'!$H$2,'K-'!$H$19,'K-'!$H$36)</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>0.1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.3</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.9</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>('K-'!$G$14,'K-'!$G$31,'K-'!$G$48)</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>30.5</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>28.3</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>22.2</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-44B8-476B-BF4E-F583DD0E0C98}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
-        <c:axId val="903675584"/>
-        <c:axId val="901880288"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="903675584"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="901880288"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="901880288"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="903675584"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -17875,6 +17936,371 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="fr-FR"/>
+              <a:t>Nombre de colonies en fonction</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="fr-FR" baseline="0"/>
+              <a:t> de K -</a:t>
+            </a:r>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="002060"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:srgbClr val="002060"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="0"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="1.6710411198600175E-4"/>
+                  <c:y val="3.1809930008748905E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="fr-FR"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>('K-'!$H$2,'K-'!$H$19,'K-'!$H$36)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>('K-'!$G$14,'K-'!$G$31,'K-'!$G$48)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>30.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>28.3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>22.2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-44B8-476B-BF4E-F583DD0E0C98}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="903675584"/>
+        <c:axId val="901880288"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="903675584"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="901880288"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="901880288"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="903675584"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart26.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="fr-FR"/>
               <a:t>Taille moyenne d'une colonie en fonction</a:t>
             </a:r>
             <a:r>
@@ -17917,24 +18343,103 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
+            <a:ln w="25400" cap="rnd">
               <a:noFill/>
+              <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:val>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="002060"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:srgbClr val="002060"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="0"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.9277340332458443E-2"/>
+                  <c:y val="-3.1469087197433653E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="fr-FR"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>('K-'!$H$2,'K-'!$H$19,'K-'!$H$36)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
               <c:f>('K-'!$H$14,'K-'!$H$31,'K-'!$H$48)</c:f>
               <c:numCache>
@@ -17951,7 +18456,8 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:yVal>
+          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-0BB3-4DEA-9571-3F0D27DB657C}"/>
@@ -17966,18 +18472,17 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
         <c:axId val="904780912"/>
         <c:axId val="783985168"/>
-      </c:barChart>
-      <c:catAx>
+      </c:scatterChart>
+      <c:valAx>
         <c:axId val="904780912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -18016,11 +18521,8 @@
         </c:txPr>
         <c:crossAx val="783985168"/>
         <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
       <c:valAx>
         <c:axId val="783985168"/>
         <c:scaling>
@@ -18075,7 +18577,7 @@
         </c:txPr>
         <c:crossAx val="904780912"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -18129,7 +18631,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart27.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="fr-FR"/>
@@ -18483,7 +18985,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart28.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="fr-FR"/>
@@ -18837,7 +19339,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart29.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="fr-FR"/>
@@ -19142,366 +19644,6 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="779640672"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="fr-FR"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart29.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="fr-FR"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="fr-FR"/>
-              <a:t>Taille moyenne d'une colonie en fonction du nombre de lignes</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="fr-FR"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="log"/>
-            <c:dispRSqr val="1"/>
-            <c:dispEq val="0"/>
-            <c:trendlineLbl>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="3.8013998250218723E-4"/>
-                  <c:y val="2.909594634004083E-2"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="fr-FR"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
-          </c:trendline>
-          <c:xVal>
-            <c:numRef>
-              <c:f>('Grid Rows (N)'!$D$19,'Grid Rows (N)'!$D$2,'Grid Rows (N)'!$D$36)</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>100</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>('Grid Rows (N)'!$H$31,'Grid Rows (N)'!$H$14,'Grid Rows (N)'!$H$48)</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>7.3456717134264409</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>7.0982748753481504</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>5.0968875337519588</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-5A4B-4B02-8D12-3E124157991B}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="973423664"/>
-        <c:axId val="904068560"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="973423664"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="904068560"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="904068560"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="973423664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -19869,7 +20011,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart30.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="fr-FR"/>
@@ -19904,15 +20046,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="fr-FR"/>
-              <a:t>Évolution</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="fr-FR" baseline="0"/>
-              <a:t> du p</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="fr-FR"/>
-              <a:t>ourcentage de blocs A voisins de blocs B en fonction de l'erreur</a:t>
+              <a:t>Taille moyenne d'une colonie en fonction du nombre de lignes</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -19950,7 +20084,367 @@
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
-        <c:scatterStyle val="smoothMarker"/>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="log"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="0"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="3.8013998250218723E-4"/>
+                  <c:y val="2.909594634004083E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="fr-FR"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>('Grid Rows (N)'!$D$19,'Grid Rows (N)'!$D$2,'Grid Rows (N)'!$D$36)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>('Grid Rows (N)'!$H$31,'Grid Rows (N)'!$H$14,'Grid Rows (N)'!$H$48)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>7.3456717134264409</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.0982748753481504</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.0968875337519588</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5A4B-4B02-8D12-3E124157991B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="973423664"/>
+        <c:axId val="904068560"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="973423664"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="904068560"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="904068560"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="973423664"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="fr-FR"/>
+              <a:t>Proportion de blocs A voisins de blocs B en fonction de l'erreur</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -19958,7 +20452,7 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:srgbClr val="7030A0"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -19973,7 +20467,7 @@
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent1"/>
+                  <a:srgbClr val="7030A0"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -20033,7 +20527,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="1"/>
+          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-5839-4874-BEF2-315DB401CB03}"/>
@@ -20242,11 +20736,11 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="fr-FR"/>
-              <a:t>Évolution</a:t>
+              <a:t>Nombre </a:t>
             </a:r>
             <a:r>
               <a:rPr lang="fr-FR" baseline="0"/>
-              <a:t> du nombre de colonies en fonction de l'erreur</a:t>
+              <a:t>de colonies en fonction de l'erreur</a:t>
             </a:r>
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
@@ -20285,7 +20779,7 @@
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
-        <c:scatterStyle val="smoothMarker"/>
+        <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -20293,7 +20787,7 @@
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:srgbClr val="7030A0"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -20308,7 +20802,7 @@
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent1"/>
+                  <a:srgbClr val="7030A0"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -20368,7 +20862,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="1"/>
+          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-9766-4507-802D-934625BC3AEF}"/>
@@ -20563,6 +21057,336 @@
 </file>
 
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Taille moyenne d'une colonie en fonction de l'erreur</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="7030A0"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:srgbClr val="7030A0"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>('Error (e)'!$J$2,'Error (e)'!$J$19,'Error (e)'!$J$36,'Error (e)'!$J$53,'Error (e)'!$J$70,'Error (e)'!$J$87)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>('Error (e)'!$H$14,'Error (e)'!$H$31,'Error (e)'!$H$48,'Error (e)'!$H$65,'Error (e)'!$H$82,'Error (e)'!$H$99)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>7.0874840732126616</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.6500997294612789</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.6616164770979456</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.4274118516209624</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.4815343774913519</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.4317876564631717</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B274-4AA8-9782-71D0498D6202}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1268722431"/>
+        <c:axId val="1341295743"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1268722431"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1341295743"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1341295743"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1268722431"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="fr-FR"/>
@@ -20885,7 +21709,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="fr-FR"/>
@@ -20962,24 +21786,77 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
+            <a:ln w="25400" cap="rnd">
               <a:noFill/>
+              <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="C00000"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:srgbClr val="C00000"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="0"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="fr-FR"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
             <c:numRef>
               <c:f>('Moves (i)'!$G$2,'Moves (i)'!$G$19,'Moves (i)'!$G$36)</c:f>
               <c:numCache>
@@ -20996,8 +21873,8 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:cat>
-          <c:val>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
               <c:f>('Moves (i)'!$L$14,'Moves (i)'!$L$31,'Moves (i)'!$L$48)</c:f>
               <c:numCache>
@@ -21014,7 +21891,8 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:yVal>
+          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-13A5-4FA1-B6D7-708CE41C388F}"/>
@@ -21029,12 +21907,10 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
         <c:axId val="700530512"/>
         <c:axId val="908485296"/>
-      </c:barChart>
-      <c:catAx>
+      </c:scatterChart>
+      <c:valAx>
         <c:axId val="700530512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
@@ -21080,11 +21956,8 @@
         </c:txPr>
         <c:crossAx val="908485296"/>
         <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
       <c:valAx>
         <c:axId val="908485296"/>
         <c:scaling>
@@ -21139,310 +22012,7 @@
         </c:txPr>
         <c:crossAx val="700530512"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="fr-FR"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="fr-FR"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="fr-FR"/>
-              <a:t>Nombre de colonies en fonction du nombre de mouvements successifs</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="fr-FR"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:numRef>
-              <c:f>('Moves (i)'!$G$2,'Moves (i)'!$G$19,'Moves (i)'!$G$36)</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>10</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>('Moves (i)'!$G$14,'Moves (i)'!$G$31,'Moves (i)'!$G$48)</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>25.9</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>118.2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>116.2</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-0A10-4D5A-A5B7-75CE9DC8EBF7}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
-        <c:axId val="896455296"/>
-        <c:axId val="709410816"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="896455296"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="709410816"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="709410816"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="896455296"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -21531,13 +22101,8 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="fr-FR"/>
-              <a:t>Taille</a:t>
+              <a:t>Nombre de colonies en fonction du nombre de mouvements successifs</a:t>
             </a:r>
-            <a:r>
-              <a:rPr lang="fr-FR" baseline="0"/>
-              <a:t> moyenne d'une colonie en fonction du nombre de mouvements successifs</a:t>
-            </a:r>
-            <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -21573,24 +22138,37 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="C00000"/>
+              </a:solidFill>
+              <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="C00000"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:srgbClr val="C00000"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
             <c:numRef>
               <c:f>('Moves (i)'!$G$2,'Moves (i)'!$G$19,'Moves (i)'!$G$36)</c:f>
               <c:numCache>
@@ -21607,28 +22185,29 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:cat>
-          <c:val>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
-              <c:f>('Moves (i)'!$H$14,'Moves (i)'!$H$31,'Moves (i)'!$H$48)</c:f>
+              <c:f>('Moves (i)'!$G$14,'Moves (i)'!$G$31,'Moves (i)'!$G$48)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>7.7870032305275938</c:v>
+                  <c:v>25.9</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.6819178241816435</c:v>
+                  <c:v>118.2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.6208390158958212</c:v>
+                  <c:v>116.2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:yVal>
+          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-531F-4778-85A8-AED9AE2DF008}"/>
+              <c16:uniqueId val="{00000000-0A10-4D5A-A5B7-75CE9DC8EBF7}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -21640,13 +22219,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
-        <c:axId val="896834112"/>
-        <c:axId val="900187984"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="896834112"/>
+        <c:axId val="896455296"/>
+        <c:axId val="709410816"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="896455296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -21689,15 +22266,12 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="900187984"/>
+        <c:crossAx val="709410816"/>
         <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
       <c:valAx>
-        <c:axId val="900187984"/>
+        <c:axId val="709410816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -21748,9 +22322,9 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="896834112"/>
+        <c:crossAx val="896455296"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -21882,24 +22456,6 @@
 </file>
 
 <file path=xl/charts/colors11.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinear" id="17">
-  <a:schemeClr val="accent4"/>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/colors12.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinear" id="17">
-  <a:schemeClr val="accent4"/>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/colors13.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinear" id="17">
-  <a:schemeClr val="accent4"/>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/colors14.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -21936,6 +22492,24 @@
     <a:lumMod val="50000"/>
     <a:lumOff val="50000"/>
   </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors12.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinear" id="17">
+  <a:schemeClr val="accent4"/>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors13.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinear" id="17">
+  <a:schemeClr val="accent4"/>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors14.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinear" id="17">
+  <a:schemeClr val="accent4"/>
 </cs:colorStyle>
 </file>
 
@@ -22497,9 +23071,12 @@
 </file>
 
 <file path=xl/charts/colors28.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="12">
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
   <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
   <a:schemeClr val="accent6"/>
   <cs:variation/>
   <cs:variation>
@@ -22575,6 +23152,43 @@
   <a:schemeClr val="accent6"/>
   <a:schemeClr val="accent5"/>
   <a:schemeClr val="accent4"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors30.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="12">
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent6"/>
   <cs:variation/>
   <cs:variation>
     <a:lumMod val="60000"/>
@@ -22688,12 +23302,6 @@
 </file>
 
 <file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinear" id="16">
-  <a:schemeClr val="accent3"/>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -22730,6 +23338,12 @@
     <a:lumMod val="50000"/>
     <a:lumOff val="50000"/>
   </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinear" id="16">
+  <a:schemeClr val="accent3"/>
 </cs:colorStyle>
 </file>
 
@@ -33880,6 +34494,509 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style30.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -37646,13 +38763,13 @@
       <xdr:col>6</xdr:col>
       <xdr:colOff>103908</xdr:colOff>
       <xdr:row>101</xdr:row>
-      <xdr:rowOff>13855</xdr:rowOff>
+      <xdr:rowOff>13856</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>1343890</xdr:colOff>
-      <xdr:row>118</xdr:row>
-      <xdr:rowOff>152399</xdr:rowOff>
+      <xdr:colOff>415636</xdr:colOff>
+      <xdr:row>117</xdr:row>
+      <xdr:rowOff>110836</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -37672,6 +38789,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>491835</xdr:colOff>
+      <xdr:row>119</xdr:row>
+      <xdr:rowOff>110836</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>270163</xdr:colOff>
+      <xdr:row>134</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Graphique 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F6E48053-FD58-4853-8B89-F6E7B1BD897E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -43056,8 +44209,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J99"/>
   <sheetViews>
-    <sheetView topLeftCell="A82" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="K109" sqref="K109"/>
+    <sheetView topLeftCell="A88" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="G131" sqref="G131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -45822,7 +46975,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView topLeftCell="A28" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="J83" sqref="J83"/>
     </sheetView>
   </sheetViews>
@@ -48154,8 +49307,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:L48"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I58" sqref="I58"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G84" sqref="G84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -53923,8 +55076,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:L48"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J73" sqref="J73"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F67" sqref="F67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
:pencil: ajout partie sur K-
</commit_message>
<xml_diff>
--- a/sample/résultats rapport + graphiques.xlsx
+++ b/sample/résultats rapport + graphiques.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Laura\cours\polytech\5a\s9\OVR - SMA\5A-SMA-Tri-Collectif\sample\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27E64C1F-1914-401F-9979-44E4F00A55F3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56FCDA94-AA0A-4DA9-A5DB-07A2B33DB91A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,13 +25,6 @@
     <sheet name="Grid Cols (M)" sheetId="10" r:id="rId10"/>
     <sheet name="Grid Rows (N)" sheetId="11" r:id="rId11"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">('Error (e)'!$G$14,'Error (e)'!$G$31,'Error (e)'!$G$48,'Error (e)'!$G$65,'Error (e)'!$G$82,'Error (e)'!$G$99)</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">('Error (e)'!$J$2,'Error (e)'!$J$19,'Error (e)'!$J$36,'Error (e)'!$J$53,'Error (e)'!$J$70,'Error (e)'!$J$87)</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">('K-'!$H$14,'K-'!$H$31,'K-'!$H$48)</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">('K-'!$H$2,'K-'!$H$19,'K-'!$H$36)</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">('K-'!$H$14,'K-'!$H$31,'K-'!$H$48)</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -17661,6 +17654,12 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="0"/>
             <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.965660542432196E-2"/>
+                  <c:y val="-2.0177165354330708E-3"/>
+                </c:manualLayout>
+              </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -55076,8 +55075,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:L48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F67" sqref="F67"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I64" sqref="I64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
:pencil: ajout partie / moves
</commit_message>
<xml_diff>
--- a/sample/résultats rapport + graphiques.xlsx
+++ b/sample/résultats rapport + graphiques.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Laura\cours\polytech\5a\s9\OVR - SMA\5A-SMA-Tri-Collectif\sample\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56FCDA94-AA0A-4DA9-A5DB-07A2B33DB91A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7789F227-0DCA-4BE8-B5C3-1169B416B936}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Agents" sheetId="1" r:id="rId1"/>
@@ -49306,8 +49306,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:L48"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G84" sqref="G84"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I55" sqref="I55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -55075,7 +55075,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:L48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A49" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="I64" sqref="I64"/>
     </sheetView>
   </sheetViews>

</xml_diff>